<commit_message>
Scripting DPLKKPS002-009 until DPLKKPS002-011 and DPLKKPS002-013
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8A30C7-B49B-4EED-8587-1ADCF038D016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E8996B-250D-4BE9-AB0A-1E2FD74FDB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,13 +145,13 @@
     <t>107.0.5304.107 (Official Build) (64-bit)</t>
   </si>
   <si>
-    <t>http://192.168.168.111/</t>
-  </si>
-  <si>
     <t>DPLK - Regression Test</t>
   </si>
   <si>
     <t>DPLK</t>
+  </si>
+  <si>
+    <t>http://192.168.168.107/</t>
   </si>
 </sst>
 </file>
@@ -208,15 +208,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -530,7 +527,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,10 +648,10 @@
       <c r="C2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -667,13 +664,13 @@
         <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Scripting DPLKINV002-003 until DPLKINV002-007
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E8996B-250D-4BE9-AB0A-1E2FD74FDB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81534A7C-6985-4AC9-AB75-0EF4068CB89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scripting DPLKINV002-023 until DPLKINV002-027
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81534A7C-6985-4AC9-AB75-0EF4068CB89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE4471A-E4E5-43F9-B709-09C5E13BE4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <t>DPLK</t>
   </si>
   <si>
-    <t>http://192.168.168.107/</t>
+    <t>http://192.168.168.111/</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scripting DPLKINV002-031 and DPLKINV003-001 until DPLKINV003-003
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE4471A-E4E5-43F9-B709-09C5E13BE4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518D7CF1-3A4D-4007-B176-4BAC438DAAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <t>DPLK</t>
   </si>
   <si>
-    <t>http://192.168.168.111/</t>
+    <t>http://192.168.168.107/</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scripting DPLKINV003-009 and DPLKINV003-013 until DPLKINV003-015
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FC12CE-450C-493F-95B4-EF10750DC29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AB176C-E1DD-40A1-85B0-9F29F39F78C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <t>DPLK</t>
   </si>
   <si>
-    <t>http://192.168.168.111/</t>
+    <t>http://192.168.168.107/</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
- 15/02/2023 -> Scripting DPLKINV121-001 until DPLKINV125-001, DPLKINV146-001 (Profile Reksa)              -> Scripting DPLKKEU001-001 until DPLKKEU005-001 (Setup Mapping Bank Pembayaran)              -> Scripting DPLKKEU013-001 and DPLKKEU015 (Entry Pembayaran Operasional)              -> Scripting DPLKKPS141-001 and DPLKKPS142-001 (Reverse Deposito)
- 16/02/2023 -> Scripting DPLKINV137-001 until DPLKINV141-001 (Dealing Ticket Deposito)
             -> Scripting DPLKKEU036-001 and DPLKKEU037-001 (Break Deposito)
             -> Scripting DPLKKEU038-001 and DPLKKEU039-001 (Jual Beli Reksadana)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AB176C-E1DD-40A1-85B0-9F29F39F78C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374BB976-9AF4-4358-9191-2B064991E54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <t>DPLK</t>
   </si>
   <si>
-    <t>http://192.168.168.107/</t>
+    <t>http://192.168.168.111/</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
     <col min="1" max="1" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.28515625" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
17/02/2023 -> Scripting DPLKINV152-001 until DPLKINV153-002 (Deviden) -> Scripting DPLKINV154-001 until DPLKINV155-002 (Dealing Ticket Reksadana) -> Re-running kepesertaan Reverse (30 kembali ke reg, 30 hapus data)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374BB976-9AF4-4358-9191-2B064991E54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226964F1-7F10-4DC6-BB51-5333F615568C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,7 +527,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
->Scripting DPLKINV126-001 until DPLKINV131-002 (Dealing Ticket Fixed Income and Dealing Ticket Order Fixed Income)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKLib_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16450FA-6163-4FE6-ADDC-5109412372FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D062E26-F7A7-475D-AB68-730782F7E0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
     <t>DPLK</t>
   </si>
   <si>
-    <t>http://192.168.168.107/</t>
+    <t>http://192.168.168.111/</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>